<commit_message>
test unitario verificando validators em src/core/category/tests/unit/domain/test_unit_validators.py
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -10109,10 +10109,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -10138,8 +10138,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10153,10 +10154,47 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10167,15 +10205,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10196,37 +10274,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -10235,55 +10282,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10346,37 +10346,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10394,13 +10382,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10418,7 +10406,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10430,13 +10430,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10448,13 +10508,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10466,67 +10520,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10568,6 +10568,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -10580,8 +10595,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10601,6 +10631,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -10615,201 +10665,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:A72"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -32208,7 +32208,7 @@
       <c r="A8" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>1331</v>
       </c>
     </row>
@@ -32725,7 +32725,7 @@
       </c>
     </row>
     <row r="73" ht="15.75" spans="1:3">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>832</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -32733,7 +32733,7 @@
       </c>
     </row>
     <row r="74" ht="15.75" spans="1:3">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>838</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -32965,7 +32965,7 @@
       </c>
     </row>
     <row r="103" ht="15.75" spans="1:3">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="2" t="s">
         <v>1024</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -33229,7 +33229,7 @@
       </c>
     </row>
     <row r="136" ht="15.75" spans="1:3">
-      <c r="A136" s="3" t="s">
+      <c r="A136" s="2" t="s">
         <v>1199</v>
       </c>
       <c r="C136" s="1" t="s">

</xml_diff>

<commit_message>
test integração verificando valiadtors em src/core/__seedwork/tests/integration/domain/test_init_validators.py
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -32741,7 +32741,7 @@
       </c>
     </row>
     <row r="75" ht="15.75" spans="1:3">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>856</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -32749,7 +32749,7 @@
       </c>
     </row>
     <row r="76" ht="15.75" spans="1:3">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>862</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -32757,7 +32757,7 @@
       </c>
     </row>
     <row r="77" ht="15.75" spans="1:3">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>869</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -32765,7 +32765,7 @@
       </c>
     </row>
     <row r="78" ht="15.75" spans="1:3">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>875</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -32797,7 +32797,7 @@
       </c>
     </row>
     <row r="82" ht="15.75" spans="1:3">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="2" t="s">
         <v>898</v>
       </c>
       <c r="C82" s="3" t="s">

</xml_diff>

<commit_message>
atualizado configurações de settings.json
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -10109,10 +10109,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -10146,6 +10146,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -10153,31 +10160,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10198,31 +10183,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10238,39 +10208,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10282,8 +10237,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10346,133 +10346,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10490,7 +10364,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10502,7 +10382,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10514,19 +10514,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10568,39 +10568,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -10616,17 +10583,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10652,161 +10628,185 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -32805,7 +32805,7 @@
       </c>
     </row>
     <row r="83" ht="15.75" spans="1:3">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>905</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -32813,7 +32813,7 @@
       </c>
     </row>
     <row r="84" ht="15.75" spans="1:3">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="2" t="s">
         <v>911</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -32821,7 +32821,7 @@
       </c>
     </row>
     <row r="85" ht="15.75" spans="1:3">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="2" t="s">
         <v>917</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -32829,7 +32829,7 @@
       </c>
     </row>
     <row r="86" ht="15.75" spans="1:3">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>923</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -32837,7 +32837,7 @@
       </c>
     </row>
     <row r="87" ht="15.75" spans="1:3">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="2" t="s">
         <v>930</v>
       </c>
       <c r="C87" s="3" t="s">

</xml_diff>

<commit_message>
criando abstração para implementação dos repositórios
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -10109,9 +10109,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
@@ -10146,6 +10146,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -10154,7 +10161,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10169,10 +10176,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10180,6 +10187,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10191,41 +10206,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10252,6 +10237,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -10261,31 +10275,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -10346,7 +10346,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10358,7 +10418,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10370,7 +10478,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10388,145 +10526,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10568,17 +10568,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10628,6 +10628,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -10638,21 +10653,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10668,145 +10668,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -32138,7 +32138,7 @@
   <sheetPr/>
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
       <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
@@ -32845,7 +32845,7 @@
       </c>
     </row>
     <row r="88" ht="15.75" spans="1:3">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>937</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -32853,7 +32853,7 @@
       </c>
     </row>
     <row r="89" ht="15.75" spans="1:3">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="2" t="s">
         <v>943</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -32885,7 +32885,7 @@
       </c>
     </row>
     <row r="93" ht="15.75" spans="1:3">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="2" t="s">
         <v>964</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -32893,7 +32893,7 @@
       </c>
     </row>
     <row r="94" ht="15.75" spans="1:3">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="2" t="s">
         <v>970</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -32901,7 +32901,7 @@
       </c>
     </row>
     <row r="95" ht="15.75" spans="1:3">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="2" t="s">
         <v>977</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -32917,7 +32917,7 @@
       </c>
     </row>
     <row r="97" ht="15.75" spans="1:3">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="2" t="s">
         <v>967</v>
       </c>
       <c r="C97" s="3" t="s">
@@ -32925,7 +32925,7 @@
       </c>
     </row>
     <row r="98" ht="15.75" spans="1:3">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="2" t="s">
         <v>974</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -32933,7 +32933,7 @@
       </c>
     </row>
     <row r="99" ht="15.75" spans="1:3">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="2" t="s">
         <v>999</v>
       </c>
       <c r="C99" s="3" t="s">

</xml_diff>

<commit_message>
test unitario verificando repositories em src/core/__seedwork/tests/unit/domain/test_unit_repositories.py
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12450" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12450" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="indice" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6791" uniqueCount="3358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6887" uniqueCount="3358">
   <si>
     <t>FULL CYCLE 3.0 
 Duração: 183h 9min - 952 VIDEOS - INÍCIO 00/00</t>
@@ -25557,8 +25557,8 @@
   <sheetPr/>
   <dimension ref="A1:E393"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="AN77" sqref="AN77"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" topLeftCell="B293" workbookViewId="0">
+      <selection activeCell="E329" sqref="E329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -30271,7 +30271,7 @@
   <sheetPr/>
   <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="DA106" sqref="DA106"/>
     </sheetView>
   </sheetViews>
@@ -32136,1128 +32136,1501 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="142.713333333333" customWidth="1"/>
-    <col min="3" max="3" width="142.713333333333" customWidth="1"/>
+    <col min="1" max="1" width="93.8533333333333" customWidth="1"/>
+    <col min="4" max="4" width="97.8133333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:3">
+    <row r="1" ht="15.75" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1"/>
+      <c r="D1" s="1" t="s">
         <v>1295</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:3">
+    <row r="2" ht="15.75" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2"/>
+      <c r="D2" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:3">
+    <row r="3" ht="15.75" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3"/>
+      <c r="D3" s="1" t="s">
         <v>1165</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:3">
+    <row r="4" ht="15.75" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4"/>
+      <c r="D4" s="3" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="5" ht="15.75" spans="1:3">
+      <c r="E4" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" spans="1:5">
       <c r="A5" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5"/>
+      <c r="D5" s="3" t="s">
         <v>1315</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" spans="1:3">
+      <c r="E5" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6"/>
+      <c r="D6" s="3" t="s">
         <v>1321</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:3">
+    <row r="7" ht="15.75" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7"/>
+      <c r="D7" s="3" t="s">
         <v>1327</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:3">
+    <row r="8" ht="15.75" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8"/>
+      <c r="D8" s="2" t="s">
         <v>1331</v>
       </c>
-    </row>
-    <row r="9" ht="15.75" spans="1:3">
+      <c r="E8" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9"/>
+      <c r="D9" s="1" t="s">
         <v>1335</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="1:3">
+    <row r="10" ht="15.75" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10"/>
+      <c r="D10" s="3" t="s">
         <v>1341</v>
       </c>
     </row>
-    <row r="11" ht="15.75" spans="1:3">
+    <row r="11" ht="15.75" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11"/>
+      <c r="D11" s="3" t="s">
         <v>1347</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:3">
+    <row r="12" ht="15.75" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12"/>
+      <c r="D12" s="3" t="s">
         <v>1352</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:3">
+    <row r="13" ht="15.75" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13"/>
+      <c r="D13" s="3" t="s">
         <v>1357</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="1:3">
+    <row r="14" ht="15.75" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14"/>
+      <c r="D14" s="1" t="s">
         <v>1363</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="1:3">
+    <row r="15" ht="15.75" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B15"/>
+      <c r="D15" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="1:3">
+    <row r="16" ht="15.75" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="B16"/>
+      <c r="D16" s="1" t="s">
         <v>1335</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="1:3">
+    <row r="17" ht="15.75" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="B17"/>
+      <c r="D17" s="3" t="s">
         <v>1378</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="1:3">
+    <row r="18" ht="15.75" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="B18"/>
+      <c r="D18" s="3" t="s">
         <v>1384</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="1:3">
+    <row r="19" ht="15.75" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19"/>
+      <c r="D19" s="3" t="s">
         <v>1390</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="1:3">
+    <row r="20" ht="15.75" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20"/>
+      <c r="D20" s="3" t="s">
         <v>1396</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="1:3">
+    <row r="21" ht="15.75" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21"/>
+      <c r="D21" s="3" t="s">
         <v>1402</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="1:3">
+    <row r="22" ht="15.75" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22"/>
+      <c r="D22" s="3" t="s">
         <v>1408</v>
       </c>
-    </row>
-    <row r="23" ht="15.75" spans="1:3">
+      <c r="E22" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23"/>
+      <c r="D23" s="3" t="s">
         <v>1414</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="1:3">
+    <row r="24" ht="15.75" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24"/>
+      <c r="D24" s="1" t="s">
         <v>1419</v>
       </c>
     </row>
-    <row r="25" ht="15.75" spans="1:3">
+    <row r="25" ht="15.75" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25"/>
+      <c r="D25" s="3" t="s">
         <v>1387</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="1:3">
+    <row r="26" ht="15.75" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26"/>
+      <c r="D26" s="3" t="s">
         <v>1426</v>
       </c>
-    </row>
-    <row r="27" ht="15.75" spans="1:3">
+      <c r="E26" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27"/>
+      <c r="D27" s="1" t="s">
         <v>1432</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="1:3">
+    <row r="28" ht="15.75" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28"/>
+      <c r="D28" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="29" ht="15.75" spans="1:3">
+    <row r="29" ht="15.75" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="B29"/>
+      <c r="D29" s="1" t="s">
         <v>1419</v>
       </c>
     </row>
-    <row r="30" ht="15.75" spans="1:3">
+    <row r="30" ht="15.75" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="B30"/>
+      <c r="D30" s="3" t="s">
         <v>1447</v>
       </c>
     </row>
-    <row r="31" ht="15.75" spans="1:3">
+    <row r="31" ht="15.75" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31"/>
+      <c r="D31" s="3" t="s">
         <v>1450</v>
       </c>
     </row>
-    <row r="32" ht="15.75" spans="1:3">
+    <row r="32" ht="15.75" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32"/>
+      <c r="D32" s="3" t="s">
         <v>1455</v>
       </c>
     </row>
-    <row r="33" ht="15.75" spans="1:3">
+    <row r="33" ht="15.75" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="B33"/>
+      <c r="D33" s="3" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="34" ht="15.75" spans="1:3">
+    <row r="34" ht="15.75" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34"/>
+      <c r="D34" s="3" t="s">
         <v>1467</v>
       </c>
     </row>
-    <row r="35" ht="15.75" spans="1:3">
+    <row r="35" ht="15.75" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="B35"/>
+      <c r="D35" s="3" t="s">
         <v>1472</v>
       </c>
-    </row>
-    <row r="36" ht="15.75" spans="1:3">
+      <c r="E35" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" spans="1:5">
       <c r="A36" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36"/>
+      <c r="D36" s="3" t="s">
         <v>1477</v>
       </c>
-    </row>
-    <row r="37" ht="15.75" spans="1:3">
+      <c r="E36" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" spans="1:5">
       <c r="A37" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="B37"/>
+      <c r="D37" s="3" t="s">
         <v>1483</v>
       </c>
-    </row>
-    <row r="38" ht="15.75" spans="1:3">
+      <c r="E37" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="B38"/>
+      <c r="D38" s="3" t="s">
         <v>1489</v>
       </c>
-    </row>
-    <row r="39" ht="15.75" spans="1:3">
+      <c r="E38" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39"/>
+      <c r="D39" s="1" t="s">
         <v>1495</v>
       </c>
     </row>
-    <row r="40" ht="15.75" spans="1:3">
+    <row r="40" ht="15.75" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40"/>
+      <c r="D40" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="41" ht="15.75" spans="1:3">
+    <row r="41" ht="15.75" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41"/>
+      <c r="D41" s="1" t="s">
         <v>1419</v>
       </c>
     </row>
-    <row r="42" ht="15.75" spans="1:3">
+    <row r="42" ht="15.75" spans="1:5">
       <c r="A42" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="B42"/>
+      <c r="D42" s="3" t="s">
         <v>1508</v>
       </c>
-    </row>
-    <row r="43" ht="15.75" spans="1:3">
+      <c r="E42" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" spans="1:4">
       <c r="A43" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="B43"/>
+      <c r="D43" s="3" t="s">
         <v>1514</v>
       </c>
     </row>
-    <row r="44" ht="15.75" spans="1:3">
+    <row r="44" ht="15.75" spans="1:5">
       <c r="A44" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44"/>
+      <c r="D44" s="3" t="s">
         <v>1520</v>
       </c>
-    </row>
-    <row r="45" ht="15.75" spans="1:3">
+      <c r="E44" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>1525</v>
       </c>
     </row>
-    <row r="46" ht="15.75" spans="1:3">
+    <row r="46" ht="15.75" spans="1:5">
       <c r="A46" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="B46"/>
+      <c r="D46" s="3" t="s">
         <v>1530</v>
       </c>
-    </row>
-    <row r="47" ht="15.75" spans="1:3">
+      <c r="E46" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" spans="1:4">
       <c r="A47" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="B47"/>
+      <c r="D47" s="3" t="s">
         <v>1536</v>
       </c>
     </row>
-    <row r="48" ht="15.75" spans="1:3">
+    <row r="48" ht="15.75" spans="1:5">
       <c r="A48" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="B48"/>
+      <c r="D48" s="3" t="s">
         <v>1542</v>
       </c>
-    </row>
-    <row r="49" ht="15.75" spans="1:3">
+      <c r="E48" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="B49" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="50" ht="15.75" spans="1:3">
+    <row r="50" ht="15.75" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="B50"/>
+      <c r="D50" s="3" t="s">
         <v>1553</v>
       </c>
     </row>
-    <row r="51" ht="15.75" spans="1:3">
+    <row r="51" ht="15.75" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>717</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="B51" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>1559</v>
       </c>
     </row>
-    <row r="52" ht="15.75" spans="1:3">
+    <row r="52" ht="15.75" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="B52"/>
+      <c r="D52" s="3" t="s">
         <v>1565</v>
       </c>
     </row>
-    <row r="53" ht="15.75" spans="1:3">
+    <row r="53" ht="15.75" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="B53"/>
+      <c r="D53" s="3" t="s">
         <v>1571</v>
       </c>
-    </row>
-    <row r="54" ht="15.75" spans="1:3">
+      <c r="E53" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54"/>
+      <c r="D54" s="1" t="s">
         <v>1576</v>
       </c>
     </row>
-    <row r="55" ht="15.75" spans="1:3">
+    <row r="55" ht="15.75" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>741</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="B55"/>
+      <c r="D55" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="56" ht="15.75" spans="1:3">
+    <row r="56" ht="15.75" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56"/>
+      <c r="D56" s="1" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="57" ht="15.75" spans="1:3">
+    <row r="57" ht="15.75" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="B57"/>
+      <c r="D57" s="3" t="s">
         <v>1586</v>
       </c>
     </row>
-    <row r="58" ht="15.75" spans="1:3">
+    <row r="58" ht="15.75" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="B58"/>
+      <c r="D58" s="3" t="s">
         <v>1591</v>
       </c>
     </row>
-    <row r="59" ht="15.75" spans="1:3">
+    <row r="59" ht="15.75" spans="1:5">
       <c r="A59" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="B59"/>
+      <c r="D59" s="3" t="s">
         <v>1597</v>
       </c>
-    </row>
-    <row r="60" ht="15.75" spans="1:3">
+      <c r="E59" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="60" ht="15.75" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>771</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="B60"/>
+      <c r="D60" s="3" t="s">
         <v>1603</v>
       </c>
     </row>
-    <row r="61" ht="15.75" spans="1:3">
+    <row r="61" ht="15.75" spans="1:5">
       <c r="A61" s="2" t="s">
         <v>777</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="B61" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>1609</v>
       </c>
-    </row>
-    <row r="62" ht="15.75" spans="1:3">
+      <c r="E61" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="B62"/>
+      <c r="D62" s="3" t="s">
         <v>1614</v>
       </c>
     </row>
-    <row r="63" ht="15.75" spans="1:3">
+    <row r="63" ht="15.75" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="B63"/>
+      <c r="D63" s="3" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="64" ht="15.75" spans="1:3">
+    <row r="64" ht="15.75" spans="1:5">
       <c r="A64" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="B64"/>
+      <c r="D64" s="3" t="s">
         <v>1626</v>
       </c>
-    </row>
-    <row r="65" ht="15.75" spans="1:3">
+      <c r="E64" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="65" ht="15.75" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="B65"/>
+      <c r="D65" s="3" t="s">
         <v>1632</v>
       </c>
     </row>
-    <row r="66" ht="15.75" spans="1:3">
+    <row r="66" ht="15.75" spans="1:5">
       <c r="A66" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="B66"/>
+      <c r="D66" s="3" t="s">
         <v>1638</v>
       </c>
-    </row>
-    <row r="67" ht="15.75" spans="1:3">
+      <c r="E66" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="67" ht="15.75" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="B67"/>
+      <c r="D67" s="3" t="s">
         <v>1644</v>
       </c>
     </row>
-    <row r="68" ht="15.75" spans="1:3">
+    <row r="68" ht="15.75" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="B68"/>
+      <c r="D68" s="3" t="s">
         <v>1650</v>
       </c>
-    </row>
-    <row r="69" ht="15.75" spans="1:3">
+      <c r="E68" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="B69"/>
+      <c r="D69" s="3" t="s">
         <v>1655</v>
       </c>
     </row>
-    <row r="70" ht="15.75" spans="1:3">
+    <row r="70" ht="15.75" spans="1:5">
       <c r="A70" s="2" t="s">
         <v>801</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="B70" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>1660</v>
       </c>
-    </row>
-    <row r="71" ht="15.75" spans="1:3">
+      <c r="E70" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="71" ht="15.75" spans="1:4">
       <c r="A71" s="2" t="s">
         <v>822</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="B71" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>1665</v>
       </c>
     </row>
-    <row r="72" ht="15.75" spans="1:3">
+    <row r="72" ht="15.75" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>826</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="B72" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>1669</v>
       </c>
     </row>
-    <row r="73" ht="15.75" spans="1:3">
+    <row r="73" ht="15.75" spans="1:4">
       <c r="A73" s="2" t="s">
         <v>832</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="B73"/>
+      <c r="D73" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="74" ht="15.75" spans="1:3">
+    <row r="74" ht="15.75" spans="1:4">
       <c r="A74" s="2" t="s">
         <v>838</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="B74"/>
+      <c r="D74" s="1" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="75" ht="15.75" spans="1:3">
+    <row r="75" ht="15.75" spans="1:5">
       <c r="A75" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="B75" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="76" ht="15.75" spans="1:3">
+      <c r="E75" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="76" ht="15.75" spans="1:5">
       <c r="A76" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="B76"/>
+      <c r="D76" s="3" t="s">
         <v>1690</v>
       </c>
-    </row>
-    <row r="77" ht="15.75" spans="1:3">
+      <c r="E76" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="77" ht="15.75" spans="1:5">
       <c r="A77" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="B77"/>
+      <c r="D77" s="3" t="s">
         <v>1695</v>
       </c>
-    </row>
-    <row r="78" ht="15.75" spans="1:3">
+      <c r="E77" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="78" ht="15.75" spans="1:5">
       <c r="A78" s="2" t="s">
         <v>875</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="B78" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>1700</v>
       </c>
-    </row>
-    <row r="79" ht="15.75" spans="1:3">
+      <c r="E78" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="79" ht="15.75" spans="1:5">
       <c r="A79" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="B79"/>
+      <c r="D79" s="3" t="s">
         <v>1705</v>
       </c>
-    </row>
-    <row r="80" ht="15.75" spans="1:3">
+      <c r="E79" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="80" ht="15.75" spans="1:5">
       <c r="A80" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="B80"/>
+      <c r="D80" s="3" t="s">
         <v>1711</v>
       </c>
-    </row>
-    <row r="81" ht="15.75" spans="1:3">
+      <c r="E80" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="81" ht="15.75" spans="1:5">
       <c r="A81" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="B81"/>
+      <c r="D81" s="3" t="s">
         <v>1717</v>
       </c>
-    </row>
-    <row r="82" ht="15.75" spans="1:3">
+      <c r="E81" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="82" ht="15.75" spans="1:5">
       <c r="A82" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="B82"/>
+      <c r="D82" s="3" t="s">
         <v>1722</v>
       </c>
-    </row>
-    <row r="83" ht="15.75" spans="1:3">
+      <c r="E82" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="83" ht="15.75" spans="1:5">
       <c r="A83" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="B83"/>
+      <c r="D83" s="3" t="s">
         <v>1727</v>
       </c>
-    </row>
-    <row r="84" ht="15.75" spans="1:3">
+      <c r="E83" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="84" ht="15.75" spans="1:5">
       <c r="A84" s="2" t="s">
         <v>911</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="B84" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>1732</v>
       </c>
-    </row>
-    <row r="85" ht="15.75" spans="1:3">
+      <c r="E84" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="85" ht="15.75" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>917</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="B85" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>1737</v>
       </c>
     </row>
-    <row r="86" ht="15.75" spans="1:3">
+    <row r="86" ht="15.75" spans="1:5">
       <c r="A86" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="B86"/>
+      <c r="D86" s="3" t="s">
         <v>1743</v>
       </c>
-    </row>
-    <row r="87" ht="15.75" spans="1:3">
+      <c r="E86" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="87" ht="15.75" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>930</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="B87"/>
+      <c r="D87" s="3" t="s">
         <v>1749</v>
       </c>
     </row>
-    <row r="88" ht="15.75" spans="1:3">
+    <row r="88" ht="15.75" spans="1:5">
       <c r="A88" s="2" t="s">
         <v>937</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="B88" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>1755</v>
       </c>
-    </row>
-    <row r="89" ht="15.75" spans="1:3">
+      <c r="E88" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="89" ht="15.75" spans="1:4">
       <c r="A89" s="2" t="s">
         <v>943</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="B89" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>1760</v>
       </c>
     </row>
-    <row r="90" ht="15.75" spans="1:3">
+    <row r="90" ht="15.75" spans="1:4">
       <c r="A90" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="B90"/>
+      <c r="D90" s="1" t="s">
         <v>1765</v>
       </c>
     </row>
-    <row r="91" ht="15.75" spans="1:3">
+    <row r="91" ht="15.75" spans="1:4">
       <c r="A91" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="B91"/>
+      <c r="D91" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="92" ht="15.75" spans="1:3">
+    <row r="92" ht="15.75" spans="1:4">
       <c r="A92" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="B92"/>
+      <c r="D92" s="1" t="s">
         <v>1737</v>
       </c>
     </row>
-    <row r="93" ht="15.75" spans="1:3">
+    <row r="93" ht="15.75" spans="1:5">
       <c r="A93" s="2" t="s">
         <v>964</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="B93" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D93" s="3" t="s">
         <v>1779</v>
       </c>
-    </row>
-    <row r="94" ht="15.75" spans="1:3">
+      <c r="E93" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="94" ht="15.75" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>970</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="B94"/>
+      <c r="D94" s="3" t="s">
         <v>1785</v>
       </c>
     </row>
-    <row r="95" ht="15.75" spans="1:3">
+    <row r="95" ht="15.75" spans="1:5">
       <c r="A95" s="2" t="s">
         <v>977</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="B95" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D95" s="3" t="s">
         <v>1791</v>
       </c>
-    </row>
-    <row r="96" ht="15.75" spans="1:3">
+      <c r="E95" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="96" ht="15.75" spans="1:4">
       <c r="A96" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="B96"/>
+      <c r="D96" s="3" t="s">
         <v>1797</v>
       </c>
     </row>
-    <row r="97" ht="15.75" spans="1:3">
+    <row r="97" ht="15.75" spans="1:5">
       <c r="A97" s="2" t="s">
         <v>967</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="B97"/>
+      <c r="D97" s="3" t="s">
         <v>1802</v>
       </c>
-    </row>
-    <row r="98" ht="15.75" spans="1:3">
+      <c r="E97" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="98" ht="15.75" spans="1:5">
       <c r="A98" s="2" t="s">
         <v>974</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="B98"/>
+      <c r="D98" s="3" t="s">
         <v>1807</v>
       </c>
-    </row>
-    <row r="99" ht="15.75" spans="1:3">
+      <c r="E98" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="99" ht="15.75" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>999</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="B99"/>
+      <c r="D99" s="3" t="s">
         <v>1813</v>
       </c>
     </row>
-    <row r="100" ht="15.75" spans="1:3">
-      <c r="A100" s="3" t="s">
+    <row r="100" ht="15.75" spans="1:4">
+      <c r="A100" s="2" t="s">
         <v>1005</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="B100" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D100" s="3" t="s">
         <v>1819</v>
       </c>
     </row>
-    <row r="101" ht="15.75" spans="1:3">
+    <row r="101" ht="15.75" spans="1:4">
       <c r="A101" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="B101" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D101" s="3" t="s">
         <v>1825</v>
       </c>
     </row>
-    <row r="102" ht="15.75" spans="1:3">
+    <row r="102" ht="15.75" spans="1:4">
       <c r="A102" s="3" t="s">
         <v>1017</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="B102" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>1830</v>
       </c>
     </row>
-    <row r="103" ht="15.75" spans="1:3">
+    <row r="103" ht="15.75" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>1024</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="B103"/>
+      <c r="D103" s="1" t="s">
         <v>1834</v>
       </c>
     </row>
-    <row r="104" ht="15.75" spans="1:3">
+    <row r="104" ht="15.75" spans="1:4">
       <c r="A104" s="1" t="s">
         <v>1030</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="B104"/>
+      <c r="D104" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="105" ht="15.75" spans="1:3">
+    <row r="105" ht="15.75" spans="1:4">
       <c r="A105" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="B105"/>
+      <c r="D105" s="1" t="s">
         <v>1737</v>
       </c>
     </row>
-    <row r="106" ht="15.75" spans="1:3">
+    <row r="106" ht="15.75" spans="1:5">
       <c r="A106" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="B106"/>
+      <c r="D106" s="3" t="s">
         <v>1849</v>
       </c>
-    </row>
-    <row r="107" ht="15.75" spans="1:3">
+      <c r="E106" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="107" ht="15.75" spans="1:5">
       <c r="A107" s="3" t="s">
         <v>1045</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="B107"/>
+      <c r="D107" s="3" t="s">
         <v>1854</v>
       </c>
-    </row>
-    <row r="108" ht="15.75" spans="1:3">
+      <c r="E107" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="108" ht="15.75" spans="1:4">
       <c r="A108" s="3" t="s">
         <v>1052</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="B108"/>
+      <c r="D108" s="3" t="s">
         <v>1859</v>
       </c>
     </row>
-    <row r="109" ht="15.75" spans="1:3">
+    <row r="109" ht="15.75" spans="1:5">
       <c r="A109" s="3" t="s">
         <v>1059</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="B109"/>
+      <c r="D109" s="3" t="s">
         <v>1865</v>
       </c>
-    </row>
-    <row r="110" ht="15.75" spans="1:3">
+      <c r="E109" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="110" ht="15.75" spans="1:4">
       <c r="A110" s="3" t="s">
         <v>1066</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="B110" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>1871</v>
       </c>
     </row>
-    <row r="111" ht="15.75" spans="1:3">
+    <row r="111" ht="15.75" spans="1:5">
       <c r="A111" s="3" t="s">
         <v>1072</v>
       </c>
-      <c r="C111" s="3" t="s">
+      <c r="B111" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>1875</v>
       </c>
-    </row>
-    <row r="112" ht="15.75" spans="1:3">
+      <c r="E111" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="112" ht="15.75" spans="1:5">
       <c r="A112" s="3" t="s">
         <v>1078</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="B112" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D112" s="3" t="s">
         <v>1879</v>
       </c>
-    </row>
-    <row r="113" ht="15.75" spans="1:3">
+      <c r="E112" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="113" ht="15.75" spans="1:4">
       <c r="A113" s="3" t="s">
         <v>1063</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="B113"/>
+      <c r="D113" s="3" t="s">
         <v>1885</v>
       </c>
     </row>
-    <row r="114" ht="15.75" spans="1:3">
+    <row r="114" ht="15.75" spans="1:4">
       <c r="A114" s="3" t="s">
         <v>1086</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="B114" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D114" s="3" t="s">
         <v>1890</v>
       </c>
     </row>
-    <row r="115" ht="15.75" spans="1:3">
+    <row r="115" ht="15.75" spans="1:4">
       <c r="A115" s="3" t="s">
         <v>1075</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="B115"/>
+      <c r="D115" s="3" t="s">
         <v>1895</v>
       </c>
     </row>
-    <row r="116" ht="15.75" spans="1:3">
+    <row r="116" ht="15.75" spans="1:5">
       <c r="A116" s="3" t="s">
         <v>1096</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="B116"/>
+      <c r="D116" s="3" t="s">
         <v>1901</v>
       </c>
-    </row>
-    <row r="117" ht="15.75" spans="1:3">
+      <c r="E116" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="117" ht="15.75" spans="1:5">
       <c r="A117" s="3" t="s">
         <v>1101</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="B117"/>
+      <c r="D117" s="3" t="s">
         <v>1907</v>
       </c>
-    </row>
-    <row r="118" ht="15.75" spans="1:3">
+      <c r="E117" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="118" ht="15.75" spans="1:4">
       <c r="A118" s="3" t="s">
         <v>1106</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="B118"/>
+      <c r="D118" s="3" t="s">
         <v>1913</v>
       </c>
     </row>
-    <row r="119" ht="15.75" spans="1:3">
+    <row r="119" ht="15.75" spans="1:4">
       <c r="A119" s="3" t="s">
         <v>1112</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="B119" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>1919</v>
       </c>
     </row>
-    <row r="120" ht="15.75" spans="1:3">
+    <row r="120" ht="15.75" spans="1:4">
       <c r="A120" s="1" t="s">
         <v>1117</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="B120"/>
+      <c r="D120" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="121" ht="15.75" spans="1:3">
+    <row r="121" ht="15.75" spans="1:4">
       <c r="A121" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="B121"/>
+      <c r="D121" s="1" t="s">
         <v>1737</v>
       </c>
     </row>
-    <row r="122" ht="15.75" spans="1:3">
+    <row r="122" ht="15.75" spans="1:5">
       <c r="A122" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="B122"/>
+      <c r="D122" s="3" t="s">
         <v>1933</v>
       </c>
-    </row>
-    <row r="123" ht="15.75" spans="1:3">
+      <c r="E122" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="123" ht="15.75" spans="1:5">
       <c r="A123" s="3" t="s">
         <v>1130</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="B123" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D123" s="3" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="124" ht="15.75" spans="1:3">
+      <c r="E123" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="124" ht="15.75" spans="1:5">
       <c r="A124" s="3" t="s">
         <v>1136</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="B124" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D124" s="3" t="s">
         <v>1945</v>
       </c>
-    </row>
-    <row r="125" ht="15.75" spans="1:3">
+      <c r="E124" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="125" ht="15.75" spans="1:5">
       <c r="A125" s="3" t="s">
         <v>1141</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="B125" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D125" s="3" t="s">
         <v>1951</v>
       </c>
-    </row>
-    <row r="126" ht="15.75" spans="1:3">
+      <c r="E125" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="126" ht="15.75" spans="1:5">
       <c r="A126" s="3" t="s">
         <v>1147</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="B126" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D126" s="3" t="s">
         <v>1956</v>
       </c>
-    </row>
-    <row r="127" ht="15.75" spans="1:3">
+      <c r="E126" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="127" ht="15.75" spans="1:5">
       <c r="A127" s="3" t="s">
         <v>1153</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="B127" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D127" s="3" t="s">
         <v>1960</v>
       </c>
-    </row>
-    <row r="128" ht="15.75" spans="1:3">
+      <c r="E127" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="128" ht="15.75" spans="1:5">
       <c r="A128" s="3" t="s">
         <v>1159</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="B128"/>
+      <c r="D128" s="3" t="s">
         <v>1965</v>
       </c>
-    </row>
-    <row r="129" ht="15.75" spans="1:3">
+      <c r="E128" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="129" ht="15.75" spans="1:5">
       <c r="A129" s="1" t="s">
         <v>1165</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="B129"/>
+      <c r="D129" s="3" t="s">
         <v>1971</v>
       </c>
-    </row>
-    <row r="130" ht="15.75" spans="1:3">
+      <c r="E129" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="130" ht="15.75" spans="1:5">
       <c r="A130" s="3" t="s">
         <v>1144</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="B130"/>
+      <c r="D130" s="3" t="s">
         <v>1977</v>
       </c>
-    </row>
-    <row r="131" ht="15.75" spans="1:3">
+      <c r="E130" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="131" ht="15.75" spans="1:5">
       <c r="A131" s="3" t="s">
         <v>1150</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="B131"/>
+      <c r="D131" s="3" t="s">
         <v>1983</v>
       </c>
-    </row>
-    <row r="132" ht="15.75" spans="1:3">
+      <c r="E131" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="132" ht="15.75" spans="1:5">
       <c r="A132" s="3" t="s">
         <v>1181</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="B132"/>
+      <c r="D132" s="3" t="s">
         <v>1989</v>
       </c>
-    </row>
-    <row r="133" ht="15.75" spans="1:3">
+      <c r="E132" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="133" ht="15.75" spans="1:5">
       <c r="A133" s="3" t="s">
         <v>1162</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="B133"/>
+      <c r="D133" s="3" t="s">
         <v>1994</v>
       </c>
-    </row>
-    <row r="134" ht="15.75" spans="1:3">
+      <c r="E133" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="134" ht="15.75" spans="1:4">
       <c r="A134" s="3" t="s">
         <v>1192</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="B134" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D134" s="1" t="s">
         <v>1999</v>
       </c>
     </row>
-    <row r="135" ht="15.75" spans="1:3">
+    <row r="135" ht="15.75" spans="1:4">
       <c r="A135" s="3" t="s">
         <v>1196</v>
       </c>
-      <c r="C135" s="1" t="s">
+      <c r="B135"/>
+      <c r="D135" s="1" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="136" ht="15.75" spans="1:3">
+    <row r="136" ht="15.75" spans="1:4">
       <c r="A136" s="2" t="s">
         <v>1199</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="B136" s="9" t="s">
+        <v>3357</v>
+      </c>
+      <c r="D136" s="1" t="s">
         <v>1737</v>
       </c>
     </row>
-    <row r="137" ht="15.75" spans="1:3">
+    <row r="137" ht="15.75" spans="1:5">
       <c r="A137" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="C137" s="3" t="s">
+      <c r="B137"/>
+      <c r="D137" s="3" t="s">
         <v>2015</v>
       </c>
-    </row>
-    <row r="138" ht="15.75" spans="1:3">
+      <c r="E137" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="138" ht="15.75" spans="1:5">
       <c r="A138" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="C138" s="3" t="s">
+      <c r="B138"/>
+      <c r="D138" s="3" t="s">
         <v>2019</v>
       </c>
-    </row>
-    <row r="139" ht="15.75" spans="1:3">
+      <c r="E138" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="139" ht="15.75" spans="1:5">
       <c r="A139" s="1" t="s">
         <v>1165</v>
       </c>
-      <c r="C139" s="3" t="s">
+      <c r="B139"/>
+      <c r="D139" s="3" t="s">
         <v>2023</v>
+      </c>
+      <c r="E139" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="140" ht="15.75" spans="1:1">
@@ -33265,9 +33638,12 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="141" ht="15.75" spans="1:1">
+    <row r="141" ht="15.75" spans="1:2">
       <c r="A141" s="3" t="s">
         <v>1225</v>
+      </c>
+      <c r="B141" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="142" ht="15.75" spans="1:1">
@@ -33275,9 +33651,12 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="143" ht="15.75" spans="1:1">
+    <row r="143" ht="15.75" spans="1:2">
       <c r="A143" s="3" t="s">
         <v>1236</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="144" ht="15.75" spans="1:1">
@@ -33285,9 +33664,12 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="145" ht="15.75" spans="1:1">
+    <row r="145" ht="15.75" spans="1:2">
       <c r="A145" s="3" t="s">
         <v>1248</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="146" ht="15.75" spans="1:1">
@@ -33295,9 +33677,12 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="147" ht="15.75" spans="1:1">
+    <row r="147" ht="15.75" spans="1:2">
       <c r="A147" s="3" t="s">
         <v>1258</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="148" ht="15.75" spans="1:1">
@@ -33305,14 +33690,20 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="149" ht="15.75" spans="1:1">
+    <row r="149" ht="15.75" spans="1:2">
       <c r="A149" s="3" t="s">
         <v>1267</v>
       </c>
-    </row>
-    <row r="150" ht="15.75" spans="1:1">
+      <c r="B149" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="150" ht="15.75" spans="1:2">
       <c r="A150" s="3" t="s">
         <v>1273</v>
+      </c>
+      <c r="B150" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="151" ht="15.75" spans="1:1">
@@ -33320,14 +33711,20 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="152" ht="15.75" spans="1:1">
+    <row r="152" ht="15.75" spans="1:2">
       <c r="A152" s="3" t="s">
         <v>1284</v>
       </c>
-    </row>
-    <row r="153" ht="15.75" spans="1:1">
+      <c r="B152" s="9" t="s">
+        <v>3357</v>
+      </c>
+    </row>
+    <row r="153" ht="15.75" spans="1:2">
       <c r="A153" s="3" t="s">
         <v>1289</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
   </sheetData>
@@ -33341,8 +33738,8 @@
   <sheetPr/>
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="C145" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -35616,8 +36013,8 @@
   <sheetPr/>
   <dimension ref="A1:A565"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="A331" workbookViewId="0">
-      <selection activeCell="E358" sqref="E358"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
criando classe para organizar os parâmetros de busca personalizados
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33162,7 +33162,7 @@
       </c>
     </row>
     <row r="107" ht="16.5" spans="1:5">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="2" t="s">
         <v>1045</v>
       </c>
       <c r="D107" s="3" t="s">
@@ -33173,7 +33173,7 @@
       </c>
     </row>
     <row r="108" ht="16.5" spans="1:4">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="2" t="s">
         <v>1052</v>
       </c>
       <c r="D108" s="3" t="s">
@@ -33181,7 +33181,7 @@
       </c>
     </row>
     <row r="109" ht="16.5" spans="1:5">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="2" t="s">
         <v>1059</v>
       </c>
       <c r="D109" s="3" t="s">
@@ -33192,7 +33192,7 @@
       </c>
     </row>
     <row r="110" ht="16.5" spans="1:4">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="2" t="s">
         <v>1066</v>
       </c>
       <c r="B110" s="9" t="s">
@@ -33396,7 +33396,7 @@
       </c>
     </row>
     <row r="128" ht="16.5" spans="1:5">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="2" t="s">
         <v>1159</v>
       </c>
       <c r="D128" s="3" t="s">

</xml_diff>

<commit_message>
classe de resultado da busca personalizada
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33203,7 +33203,7 @@
       </c>
     </row>
     <row r="111" ht="16.5" spans="1:5">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="2" t="s">
         <v>1072</v>
       </c>
       <c r="B111" s="9" t="s">

</xml_diff>

<commit_message>
trabalhando repositório e validação da entidade Categoria
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33217,7 +33217,7 @@
       </c>
     </row>
     <row r="112" ht="16.5" spans="1:5">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="2" t="s">
         <v>1078</v>
       </c>
       <c r="B112" s="9" t="s">
@@ -33231,7 +33231,7 @@
       </c>
     </row>
     <row r="113" ht="16.5" spans="1:4">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>1063</v>
       </c>
       <c r="D113" s="3" t="s">
@@ -33239,7 +33239,7 @@
       </c>
     </row>
     <row r="114" ht="16.5" spans="1:4">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="2" t="s">
         <v>1086</v>
       </c>
       <c r="B114" s="9" t="s">
@@ -33250,7 +33250,7 @@
       </c>
     </row>
     <row r="115" ht="16.5" spans="1:4">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="2" t="s">
         <v>1075</v>
       </c>
       <c r="D115" s="3" t="s">
@@ -33258,7 +33258,7 @@
       </c>
     </row>
     <row r="116" ht="16.5" spans="1:5">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="2" t="s">
         <v>1096</v>
       </c>
       <c r="D116" s="3" t="s">
@@ -33269,7 +33269,7 @@
       </c>
     </row>
     <row r="117" ht="16.5" spans="1:5">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="2" t="s">
         <v>1101</v>
       </c>
       <c r="D117" s="3" t="s">
@@ -33280,7 +33280,7 @@
       </c>
     </row>
     <row r="118" ht="16.5" spans="1:4">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="2" t="s">
         <v>1106</v>
       </c>
       <c r="D118" s="3" t="s">
@@ -33288,7 +33288,7 @@
       </c>
     </row>
     <row r="119" ht="16.5" spans="1:4">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="2" t="s">
         <v>1112</v>
       </c>
       <c r="B119" s="9" t="s">

</xml_diff>

<commit_message>
criando lógica do caso de uso de criação de categoria
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -25557,8 +25557,8 @@
   <sheetPr/>
   <dimension ref="A1:E393"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" topLeftCell="B293" workbookViewId="0">
-      <selection activeCell="E329" sqref="E329"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -30271,8 +30271,8 @@
   <sheetPr/>
   <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="DA106" sqref="DA106"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33326,7 +33326,7 @@
       </c>
     </row>
     <row r="123" ht="16.5" spans="1:5">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="2" t="s">
         <v>1130</v>
       </c>
       <c r="B123" s="9" t="s">
@@ -33340,7 +33340,7 @@
       </c>
     </row>
     <row r="124" ht="16.5" spans="1:5">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="2" t="s">
         <v>1136</v>
       </c>
       <c r="B124" s="9" t="s">
@@ -33354,7 +33354,7 @@
       </c>
     </row>
     <row r="125" ht="16.5" spans="1:5">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="2" t="s">
         <v>1141</v>
       </c>
       <c r="B125" s="9" t="s">
@@ -33368,7 +33368,7 @@
       </c>
     </row>
     <row r="126" ht="16.5" spans="1:5">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="2" t="s">
         <v>1147</v>
       </c>
       <c r="B126" s="9" t="s">
@@ -33382,7 +33382,7 @@
       </c>
     </row>
     <row r="127" ht="16.5" spans="1:5">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="2" t="s">
         <v>1153</v>
       </c>
       <c r="B127" s="9" t="s">
@@ -33418,7 +33418,7 @@
       </c>
     </row>
     <row r="130" ht="16.5" spans="1:5">
-      <c r="A130" s="3" t="s">
+      <c r="A130" s="2" t="s">
         <v>1144</v>
       </c>
       <c r="D130" s="3" t="s">
@@ -33429,7 +33429,7 @@
       </c>
     </row>
     <row r="131" ht="16.5" spans="1:5">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="2" t="s">
         <v>1150</v>
       </c>
       <c r="D131" s="3" t="s">
@@ -33440,7 +33440,7 @@
       </c>
     </row>
     <row r="132" ht="16.5" spans="1:5">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="2" t="s">
         <v>1181</v>
       </c>
       <c r="D132" s="3" t="s">
@@ -33451,7 +33451,7 @@
       </c>
     </row>
     <row r="133" ht="16.5" spans="1:5">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="2" t="s">
         <v>1162</v>
       </c>
       <c r="D133" s="3" t="s">
@@ -33629,8 +33629,8 @@
   <sheetPr/>
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="G145" sqref="G145"/>
+    <sheetView zoomScale="25" zoomScaleNormal="25" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
criando caso de uso para pegar uma categoria
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -10109,9 +10109,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
@@ -10138,6 +10138,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -10152,47 +10160,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10206,8 +10175,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10215,7 +10216,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10237,24 +10238,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10268,7 +10260,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10277,13 +10284,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10352,7 +10352,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10364,7 +10376,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10376,7 +10442,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10388,7 +10460,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10400,13 +10490,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10424,109 +10520,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10568,6 +10568,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -10587,7 +10596,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10607,6 +10616,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -10618,26 +10647,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10656,160 +10665,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33462,7 +33462,7 @@
       </c>
     </row>
     <row r="134" ht="16.5" spans="1:4">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="2" t="s">
         <v>1192</v>
       </c>
       <c r="B134" s="9" t="s">
@@ -33473,7 +33473,7 @@
       </c>
     </row>
     <row r="135" ht="16.5" spans="1:4">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="2" t="s">
         <v>1196</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -33525,12 +33525,12 @@
       </c>
     </row>
     <row r="140" ht="16.5" spans="1:1">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="2" t="s">
         <v>1220</v>
       </c>
     </row>
     <row r="141" ht="16.5" spans="1:2">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="2" t="s">
         <v>1225</v>
       </c>
       <c r="B141" s="9" t="s">
@@ -33538,7 +33538,7 @@
       </c>
     </row>
     <row r="142" ht="16.5" spans="1:1">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="2" t="s">
         <v>1230</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criando mappers para gerar outputs
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33543,7 +33543,7 @@
       </c>
     </row>
     <row r="143" ht="16.5" spans="1:2">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="2" t="s">
         <v>1236</v>
       </c>
       <c r="B143" s="9" t="s">
@@ -33551,7 +33551,7 @@
       </c>
     </row>
     <row r="144" ht="16.5" spans="1:1">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="2" t="s">
         <v>1242</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criando abstração para os casos de usos
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33556,7 +33556,7 @@
       </c>
     </row>
     <row r="145" ht="16.5" spans="1:2">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="2" t="s">
         <v>1248</v>
       </c>
       <c r="B145" s="9" t="s">
@@ -33564,7 +33564,7 @@
       </c>
     </row>
     <row r="146" ht="16.5" spans="1:1">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="2" t="s">
         <v>1254</v>
       </c>
     </row>

</xml_diff>

<commit_message>
teste abstração para input e output de listagem de casos de uso
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33590,7 +33590,7 @@
       </c>
     </row>
     <row r="150" ht="15.75" spans="1:2">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="2" t="s">
         <v>1273</v>
       </c>
       <c r="B150" s="9" t="s">
@@ -33598,7 +33598,7 @@
       </c>
     </row>
     <row r="151" ht="15.75" spans="1:1">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="2" t="s">
         <v>1279</v>
       </c>
     </row>

</xml_diff>

<commit_message>
organizando o projeto Django e Core pastas dependências dockerfile e ambiente
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14340" windowHeight="12270" firstSheet="2" activeTab="6"/>
+    <workbookView windowWidth="14340" windowHeight="12270" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="indice" sheetId="1" r:id="rId1"/>
@@ -30271,7 +30271,7 @@
   <sheetPr/>
   <dimension ref="A1:C204"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A161" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32176,7 +32176,7 @@
       <c r="A4" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>1310</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -32187,7 +32187,7 @@
       <c r="A5" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>1315</v>
       </c>
       <c r="E5" s="9" t="s">
@@ -32198,7 +32198,7 @@
       <c r="A6" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>1321</v>
       </c>
     </row>
@@ -32206,7 +32206,7 @@
       <c r="A7" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>1327</v>
       </c>
     </row>
@@ -32233,7 +32233,7 @@
       <c r="A10" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>1341</v>
       </c>
     </row>
@@ -32241,7 +32241,7 @@
       <c r="A11" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>1347</v>
       </c>
     </row>
@@ -32249,7 +32249,7 @@
       <c r="A12" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>1352</v>
       </c>
     </row>
@@ -32257,7 +32257,7 @@
       <c r="A13" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>1357</v>
       </c>
     </row>
@@ -32289,7 +32289,7 @@
       <c r="A17" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>1378</v>
       </c>
     </row>
@@ -32297,7 +32297,7 @@
       <c r="A18" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>1384</v>
       </c>
     </row>
@@ -32305,7 +32305,7 @@
       <c r="A19" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>1390</v>
       </c>
     </row>
@@ -32313,7 +32313,7 @@
       <c r="A20" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>1396</v>
       </c>
     </row>
@@ -32321,7 +32321,7 @@
       <c r="A21" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>1402</v>
       </c>
     </row>
@@ -32329,7 +32329,7 @@
       <c r="A22" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>1408</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -33603,7 +33603,7 @@
       </c>
     </row>
     <row r="152" ht="15.75" spans="1:2">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="2" t="s">
         <v>1284</v>
       </c>
       <c r="B152" s="9" t="s">
@@ -33611,7 +33611,7 @@
       </c>
     </row>
     <row r="153" ht="15.75" spans="1:2">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="2" t="s">
         <v>1289</v>
       </c>
       <c r="B153" s="9" t="s">

</xml_diff>

<commit_message>
teste unitarios em controller api
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32431,7 +32431,7 @@
       <c r="A34" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>1467</v>
       </c>
     </row>
@@ -32439,7 +32439,7 @@
       <c r="A35" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>1472</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -32450,7 +32450,7 @@
       <c r="A36" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>1477</v>
       </c>
       <c r="E36" s="9" t="s">
@@ -32461,7 +32461,7 @@
       <c r="A37" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>1483</v>
       </c>
       <c r="E37" s="9" t="s">
@@ -32472,7 +32472,7 @@
       <c r="A38" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>1489</v>
       </c>
       <c r="E38" s="9" t="s">
@@ -32507,7 +32507,7 @@
       <c r="A42" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>1508</v>
       </c>
       <c r="E42" s="9" t="s">

</xml_diff>

<commit_message>
criando API Rest de Categoria In Memory
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -10109,10 +10109,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -10146,6 +10146,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -10154,45 +10169,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -10214,10 +10191,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10236,7 +10214,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -10244,8 +10221,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10260,17 +10246,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10283,9 +10261,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -10346,31 +10346,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10388,6 +10376,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -10400,13 +10394,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10418,31 +10496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10454,43 +10508,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10502,31 +10526,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10568,20 +10568,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10601,6 +10598,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -10612,17 +10627,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10644,169 +10648,165 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="C31" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32518,7 +32518,7 @@
       <c r="A43" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>1514</v>
       </c>
     </row>
@@ -32526,7 +32526,7 @@
       <c r="A44" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>1520</v>
       </c>
       <c r="E44" s="9" t="s">
@@ -32540,7 +32540,7 @@
       <c r="B45" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="2" t="s">
         <v>1525</v>
       </c>
     </row>
@@ -32548,7 +32548,7 @@
       <c r="A46" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>1530</v>
       </c>
       <c r="E46" s="9" t="s">
@@ -32559,7 +32559,7 @@
       <c r="A47" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="2" t="s">
         <v>1536</v>
       </c>
     </row>
@@ -32567,7 +32567,7 @@
       <c r="A48" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>1542</v>
       </c>
       <c r="E48" s="9" t="s">
@@ -32589,7 +32589,7 @@
       <c r="A50" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>1553</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criando tests model do Django ORM para categoria
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32139,7 +32139,7 @@
   <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32600,7 +32600,7 @@
       <c r="B51" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>1559</v>
       </c>
     </row>

</xml_diff>

<commit_message>
teste mapeador de entidade para model
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32139,7 +32139,7 @@
   <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C45" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32727,7 +32727,7 @@
       <c r="A65" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>1632</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implementado metodos insert, find_by_id, find_all, update, delete e search em repositories
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C45" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32735,7 +32735,7 @@
       <c r="A66" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>1638</v>
       </c>
       <c r="E66" s="9" t="s">
@@ -32746,7 +32746,7 @@
       <c r="A67" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>1644</v>
       </c>
     </row>
@@ -32754,7 +32754,7 @@
       <c r="A68" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>1650</v>
       </c>
       <c r="E68" s="9" t="s">
@@ -32765,7 +32765,7 @@
       <c r="A69" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="2" t="s">
         <v>1655</v>
       </c>
     </row>
@@ -32776,7 +32776,7 @@
       <c r="B70" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>1660</v>
       </c>
       <c r="E70" s="9" t="s">
@@ -32790,7 +32790,7 @@
       <c r="B71" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>1665</v>
       </c>
     </row>
@@ -32828,7 +32828,7 @@
       <c r="B75" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" s="2" t="s">
         <v>1684</v>
       </c>
       <c r="E75" s="9" t="s">

</xml_diff>

<commit_message>
testes unitarios de repositories em test_unit_repositories
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="C55" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="C60" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32839,7 +32839,7 @@
       <c r="A76" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="2" t="s">
         <v>1690</v>
       </c>
       <c r="E76" s="9" t="s">
@@ -32850,7 +32850,7 @@
       <c r="A77" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="2" t="s">
         <v>1695</v>
       </c>
       <c r="E77" s="9" t="s">
@@ -32864,7 +32864,7 @@
       <c r="B78" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="2" t="s">
         <v>1700</v>
       </c>
       <c r="E78" s="9" t="s">
@@ -32875,7 +32875,7 @@
       <c r="A79" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" s="2" t="s">
         <v>1705</v>
       </c>
       <c r="E79" s="9" t="s">

</xml_diff>

<commit_message>
criado serializer para validar previamente dados da categoria
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C66" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C86" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -32955,7 +32955,7 @@
       <c r="A86" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="2" t="s">
         <v>1743</v>
       </c>
       <c r="E86" s="9" t="s">
@@ -32966,7 +32966,7 @@
       <c r="A87" s="2" t="s">
         <v>930</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" s="2" t="s">
         <v>1749</v>
       </c>
     </row>
@@ -32977,7 +32977,7 @@
       <c r="B88" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="2" t="s">
         <v>1755</v>
       </c>
       <c r="E88" s="9" t="s">
@@ -32991,7 +32991,7 @@
       <c r="B89" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="2" t="s">
         <v>1760</v>
       </c>
     </row>
@@ -33026,7 +33026,7 @@
       <c r="B93" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" s="2" t="s">
         <v>1779</v>
       </c>
       <c r="E93" s="9" t="s">

</xml_diff>

<commit_message>
criado fixtures de categories em categories_api_fixture
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C89" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33037,7 +33037,7 @@
       <c r="A94" s="2" t="s">
         <v>970</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="2" t="s">
         <v>1785</v>
       </c>
     </row>
@@ -33048,7 +33048,7 @@
       <c r="B95" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D95" s="2" t="s">
         <v>1791</v>
       </c>
       <c r="E95" s="9" t="s">
@@ -33059,7 +33059,7 @@
       <c r="A96" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D96" s="2" t="s">
         <v>1797</v>
       </c>
     </row>
@@ -33067,7 +33067,7 @@
       <c r="A97" s="2" t="s">
         <v>967</v>
       </c>
-      <c r="D97" s="3" t="s">
+      <c r="D97" s="2" t="s">
         <v>1802</v>
       </c>
       <c r="E97" s="9" t="s">
@@ -33078,7 +33078,7 @@
       <c r="A98" s="2" t="s">
         <v>974</v>
       </c>
-      <c r="D98" s="3" t="s">
+      <c r="D98" s="2" t="s">
         <v>1807</v>
       </c>
       <c r="E98" s="9" t="s">
@@ -33089,7 +33089,7 @@
       <c r="A99" s="2" t="s">
         <v>999</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="D99" s="2" t="s">
         <v>1813</v>
       </c>
     </row>
@@ -33100,7 +33100,7 @@
       <c r="B100" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="2" t="s">
         <v>1819</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criado helpers, e teste de integração de api test_int_common_methods
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C89" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C101" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33111,7 +33111,7 @@
       <c r="B101" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D101" s="3" t="s">
+      <c r="D101" s="2" t="s">
         <v>1825</v>
       </c>
     </row>
@@ -33122,7 +33122,7 @@
       <c r="B102" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="2" t="s">
         <v>1830</v>
       </c>
     </row>
@@ -33154,7 +33154,7 @@
       <c r="A106" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="D106" s="2" t="s">
         <v>1849</v>
       </c>
       <c r="E106" s="9" t="s">
@@ -33165,7 +33165,7 @@
       <c r="A107" s="2" t="s">
         <v>1045</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="2" t="s">
         <v>1854</v>
       </c>
       <c r="E107" s="9" t="s">
@@ -33176,7 +33176,7 @@
       <c r="A108" s="2" t="s">
         <v>1052</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="2" t="s">
         <v>1859</v>
       </c>
     </row>
@@ -33184,7 +33184,7 @@
       <c r="A109" s="2" t="s">
         <v>1059</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="D109" s="2" t="s">
         <v>1865</v>
       </c>
       <c r="E109" s="9" t="s">
@@ -33198,7 +33198,7 @@
       <c r="B110" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="D110" s="2" t="s">
         <v>1871</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criado testes de integração da api em src/core/category/tests/integration/infra/django_app/api/**
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6887" uniqueCount="3358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6888" uniqueCount="3358">
   <si>
     <t>FULL CYCLE 3.0 
 Duração: 183h 9min - 952 VIDEOS - INÍCIO 00/00</t>
@@ -32139,7 +32139,7 @@
   <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C101" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33209,7 +33209,7 @@
       <c r="B111" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="2" t="s">
         <v>1875</v>
       </c>
       <c r="E111" s="9" t="s">
@@ -33223,7 +33223,7 @@
       <c r="B112" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D112" s="2" t="s">
         <v>1879</v>
       </c>
       <c r="E112" s="9" t="s">
@@ -33234,7 +33234,7 @@
       <c r="A113" s="2" t="s">
         <v>1063</v>
       </c>
-      <c r="D113" s="3" t="s">
+      <c r="D113" s="2" t="s">
         <v>1885</v>
       </c>
     </row>
@@ -33279,12 +33279,15 @@
         <v>3357</v>
       </c>
     </row>
-    <row r="118" ht="16.5" spans="1:4">
+    <row r="118" ht="16.5" spans="1:5">
       <c r="A118" s="2" t="s">
         <v>1106</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>1913</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>3357</v>
       </c>
     </row>
     <row r="119" ht="16.5" spans="1:4">

</xml_diff>

<commit_message>
criando serializador para apresentar coleção de categorias
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C101" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C110" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33245,7 +33245,7 @@
       <c r="B114" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="D114" s="2" t="s">
         <v>1890</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criado testes unitarios serializers em src/core/__seedwork/tests/unit/infra/django_app/test_unit_serializers.py
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32139,7 +32139,7 @@
   <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C110" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33253,7 +33253,7 @@
       <c r="A115" s="2" t="s">
         <v>1075</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D115" s="2" t="s">
         <v>1895</v>
       </c>
     </row>
@@ -33261,7 +33261,7 @@
       <c r="A116" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="D116" s="2" t="s">
         <v>1901</v>
       </c>
       <c r="E116" s="9" t="s">

</xml_diff>

<commit_message>
criado dados de testes de entitdades entities_faker_builder
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C110" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C101" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33272,7 +33272,7 @@
       <c r="A117" s="2" t="s">
         <v>1101</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="D117" s="2" t="s">
         <v>1907</v>
       </c>
       <c r="E117" s="9" t="s">
@@ -33283,7 +33283,7 @@
       <c r="A118" s="2" t="s">
         <v>1106</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="2" t="s">
         <v>1913</v>
       </c>
       <c r="E118" s="9" t="s">

</xml_diff>

<commit_message>
consolidando tests category resource
</commit_message>
<xml_diff>
--- a/doc/CRONOGRAMA_FULL_CYCLE.xlsx
+++ b/doc/CRONOGRAMA_FULL_CYCLE.xlsx
@@ -32138,8 +32138,8 @@
   <sheetPr/>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C101" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C125" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14074074074074" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -33321,7 +33321,7 @@
       <c r="A122" s="1" t="s">
         <v>984</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D122" s="2" t="s">
         <v>1933</v>
       </c>
       <c r="E122" s="9" t="s">
@@ -33335,7 +33335,7 @@
       <c r="B123" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="2" t="s">
         <v>1939</v>
       </c>
       <c r="E123" s="9" t="s">
@@ -33349,7 +33349,7 @@
       <c r="B124" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D124" s="3" t="s">
+      <c r="D124" s="2" t="s">
         <v>1945</v>
       </c>
       <c r="E124" s="9" t="s">
@@ -33363,7 +33363,7 @@
       <c r="B125" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="D125" s="2" t="s">
         <v>1951</v>
       </c>
       <c r="E125" s="9" t="s">
@@ -33377,7 +33377,7 @@
       <c r="B126" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="D126" s="2" t="s">
         <v>1956</v>
       </c>
       <c r="E126" s="9" t="s">
@@ -33391,7 +33391,7 @@
       <c r="B127" s="9" t="s">
         <v>3357</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D127" s="2" t="s">
         <v>1960</v>
       </c>
       <c r="E127" s="9" t="s">
@@ -33402,7 +33402,7 @@
       <c r="A128" s="2" t="s">
         <v>1159</v>
       </c>
-      <c r="D128" s="3" t="s">
+      <c r="D128" s="2" t="s">
         <v>1965</v>
       </c>
       <c r="E128" s="9" t="s">
@@ -33413,7 +33413,7 @@
       <c r="A129" s="1" t="s">
         <v>1165</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="D129" s="2" t="s">
         <v>1971</v>
       </c>
       <c r="E129" s="9" t="s">
@@ -33424,7 +33424,7 @@
       <c r="A130" s="2" t="s">
         <v>1144</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D130" s="2" t="s">
         <v>1977</v>
       </c>
       <c r="E130" s="9" t="s">
@@ -33435,7 +33435,7 @@
       <c r="A131" s="2" t="s">
         <v>1150</v>
       </c>
-      <c r="D131" s="3" t="s">
+      <c r="D131" s="2" t="s">
         <v>1983</v>
       </c>
       <c r="E131" s="9" t="s">
@@ -33446,7 +33446,7 @@
       <c r="A132" s="2" t="s">
         <v>1181</v>
       </c>
-      <c r="D132" s="3" t="s">
+      <c r="D132" s="2" t="s">
         <v>1989</v>
       </c>
       <c r="E132" s="9" t="s">
@@ -33457,7 +33457,7 @@
       <c r="A133" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="D133" s="2" t="s">
         <v>1994</v>
       </c>
       <c r="E133" s="9" t="s">
@@ -33498,7 +33498,7 @@
       <c r="A137" s="1" t="s">
         <v>1204</v>
       </c>
-      <c r="D137" s="3" t="s">
+      <c r="D137" s="2" t="s">
         <v>2015</v>
       </c>
       <c r="E137" s="9" t="s">
@@ -33509,7 +33509,7 @@
       <c r="A138" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D138" s="3" t="s">
+      <c r="D138" s="2" t="s">
         <v>2019</v>
       </c>
       <c r="E138" s="9" t="s">
@@ -33520,7 +33520,7 @@
       <c r="A139" s="1" t="s">
         <v>1165</v>
       </c>
-      <c r="D139" s="3" t="s">
+      <c r="D139" s="2" t="s">
         <v>2023</v>
       </c>
       <c r="E139" s="9" t="s">

</xml_diff>